<commit_message>
add tree test case on the authentication -> login file ...
</commit_message>
<xml_diff>
--- a/test_case/authentication/login.xlsx
+++ b/test_case/authentication/login.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>Test Scenario: Login</t>
   </si>
@@ -144,6 +144,43 @@
 2. 2. Leave the password field blank.
 3. Leave the password field blank.
 4. Click "Sign In".</t>
+  </si>
+  <si>
+    <t>QWZ-WEB-ALG-007</t>
+  </si>
+  <si>
+    <t>Email Format Validation</t>
+  </si>
+  <si>
+    <t>1. Enter an invalid email format (e.g., user@, user.com).
+2. Click "Sign In" or tab out of the field.</t>
+  </si>
+  <si>
+    <t>A validation error appears (e.g., "Please enter a valid email address").</t>
+  </si>
+  <si>
+    <t>QWZ-WEB-ALG-008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Forgot Password?" Link Functionality </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click the "Forgot Password?" link. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is redirected to the password reset request page. </t>
+  </si>
+  <si>
+    <t>QWZ-WEB-ALG-009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Sign Up" Link Functionality </t>
+  </si>
+  <si>
+    <t>1. Click the "Sign up" link.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is redirected to the user registration page. </t>
   </si>
 </sst>
 </file>
@@ -891,7 +928,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -944,9 +981,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1501,82 +1535,82 @@
     </dxf>
   </dxfs>
   <tableStyles count="16">
-    <tableStyle name="Template-style" pivot="0" count="3" xr9:uid="{EFE090BD-2A7D-4B44-8E7D-1178713EE243}">
+    <tableStyle name="Template-style" pivot="0" count="3" xr9:uid="{B75DADE6-5E0B-4719-AEA3-B029AC9AFF86}">
       <tableStyleElement type="headerRow" dxfId="9"/>
       <tableStyleElement type="firstRowStripe" dxfId="8"/>
       <tableStyleElement type="secondRowStripe" dxfId="7"/>
     </tableStyle>
-    <tableStyle name="1419-style" pivot="0" count="3" xr9:uid="{9413B18D-9C00-4B2A-90EC-90A9EB148431}">
+    <tableStyle name="1419-style" pivot="0" count="3" xr9:uid="{969723E0-A6E3-43AA-8297-E90CFC4B9061}">
       <tableStyleElement type="headerRow" dxfId="12"/>
       <tableStyleElement type="firstRowStripe" dxfId="11"/>
       <tableStyleElement type="secondRowStripe" dxfId="10"/>
     </tableStyle>
-    <tableStyle name="2147-style" pivot="0" count="3" xr9:uid="{2ECDC827-4951-4E81-8D3C-5DC2FCC0D742}">
+    <tableStyle name="2147-style" pivot="0" count="3" xr9:uid="{A68DBC02-D8C7-49B0-A4DB-F4327F061C54}">
       <tableStyleElement type="headerRow" dxfId="15"/>
       <tableStyleElement type="firstRowStripe" dxfId="14"/>
       <tableStyleElement type="secondRowStripe" dxfId="13"/>
     </tableStyle>
-    <tableStyle name="2170-style" pivot="0" count="3" xr9:uid="{5F180D72-E77E-470F-BE25-F0BA3DB24146}">
+    <tableStyle name="2170-style" pivot="0" count="3" xr9:uid="{88D28942-0153-4B35-B21D-499DEE0F30F3}">
       <tableStyleElement type="headerRow" dxfId="18"/>
       <tableStyleElement type="firstRowStripe" dxfId="17"/>
       <tableStyleElement type="secondRowStripe" dxfId="16"/>
     </tableStyle>
-    <tableStyle name="2177-style" pivot="0" count="3" xr9:uid="{274CF178-1A4B-4C03-9D52-72C48B228951}">
+    <tableStyle name="2177-style" pivot="0" count="3" xr9:uid="{8AC6B7C2-0C7E-442B-8A6B-7B5EA1327B18}">
       <tableStyleElement type="headerRow" dxfId="21"/>
       <tableStyleElement type="firstRowStripe" dxfId="20"/>
       <tableStyleElement type="secondRowStripe" dxfId="19"/>
     </tableStyle>
-    <tableStyle name="2253-style" pivot="0" count="3" xr9:uid="{DDA8075F-DA13-4A4E-9D23-B55D9AA057F1}">
+    <tableStyle name="2253-style" pivot="0" count="3" xr9:uid="{58B411DD-B8F7-479E-90D0-B2D3E33A4FD6}">
       <tableStyleElement type="headerRow" dxfId="24"/>
       <tableStyleElement type="firstRowStripe" dxfId="23"/>
       <tableStyleElement type="secondRowStripe" dxfId="22"/>
     </tableStyle>
-    <tableStyle name="2255-style" pivot="0" count="3" xr9:uid="{0DABDF66-4B5E-41C5-97BF-C4718F0B1FB8}">
+    <tableStyle name="2255-style" pivot="0" count="3" xr9:uid="{6E7EE1AB-DAC4-4353-AED6-582652EEB5B9}">
       <tableStyleElement type="headerRow" dxfId="27"/>
       <tableStyleElement type="firstRowStripe" dxfId="26"/>
       <tableStyleElement type="secondRowStripe" dxfId="25"/>
     </tableStyle>
-    <tableStyle name="2274-style" pivot="0" count="3" xr9:uid="{F490831E-732A-4D21-ABC2-24FF4197595F}">
+    <tableStyle name="2274-style" pivot="0" count="3" xr9:uid="{E4D5BF46-48EE-4C4E-901B-13A7B068CAC0}">
       <tableStyleElement type="headerRow" dxfId="30"/>
       <tableStyleElement type="firstRowStripe" dxfId="29"/>
       <tableStyleElement type="secondRowStripe" dxfId="28"/>
     </tableStyle>
-    <tableStyle name="2277-style" pivot="0" count="3" xr9:uid="{E637CD9E-DC21-4C13-8642-B6A852B4E91C}">
+    <tableStyle name="2277-style" pivot="0" count="3" xr9:uid="{5F8C80B7-9AB5-412F-BE77-79A47736F936}">
       <tableStyleElement type="headerRow" dxfId="33"/>
       <tableStyleElement type="firstRowStripe" dxfId="32"/>
       <tableStyleElement type="secondRowStripe" dxfId="31"/>
     </tableStyle>
-    <tableStyle name="2279-style" pivot="0" count="3" xr9:uid="{3D1A992A-4F35-42A4-AF84-E2CABD173B08}">
+    <tableStyle name="2279-style" pivot="0" count="3" xr9:uid="{4C8D597A-4DD9-48A6-95FC-B4A7FD02F8A3}">
       <tableStyleElement type="headerRow" dxfId="36"/>
       <tableStyleElement type="firstRowStripe" dxfId="35"/>
       <tableStyleElement type="secondRowStripe" dxfId="34"/>
     </tableStyle>
-    <tableStyle name="2280-style" pivot="0" count="3" xr9:uid="{211591E1-8BDE-4FB4-867A-12F31F23BE00}">
+    <tableStyle name="2280-style" pivot="0" count="3" xr9:uid="{CDC34ECC-88F3-4301-9877-97B8079E8694}">
       <tableStyleElement type="headerRow" dxfId="39"/>
       <tableStyleElement type="firstRowStripe" dxfId="38"/>
       <tableStyleElement type="secondRowStripe" dxfId="37"/>
     </tableStyle>
-    <tableStyle name="2283-style" pivot="0" count="3" xr9:uid="{D27A3AE9-89E4-4AC4-8AB6-927B2EAA1B0C}">
+    <tableStyle name="2283-style" pivot="0" count="3" xr9:uid="{AA25F465-CA67-4388-A541-638B11F91E8C}">
       <tableStyleElement type="headerRow" dxfId="42"/>
       <tableStyleElement type="firstRowStripe" dxfId="41"/>
       <tableStyleElement type="secondRowStripe" dxfId="40"/>
     </tableStyle>
-    <tableStyle name="2285-style" pivot="0" count="3" xr9:uid="{C576CFDF-62FF-4D64-86D4-FB9AC1E0EEE9}">
+    <tableStyle name="2285-style" pivot="0" count="3" xr9:uid="{B82F4FBA-4DA0-4131-AC7E-327245237C55}">
       <tableStyleElement type="headerRow" dxfId="45"/>
       <tableStyleElement type="firstRowStripe" dxfId="44"/>
       <tableStyleElement type="secondRowStripe" dxfId="43"/>
     </tableStyle>
-    <tableStyle name="2287-style" pivot="0" count="3" xr9:uid="{06F988A4-F628-48F4-964D-A5AC9A22E891}">
+    <tableStyle name="2287-style" pivot="0" count="3" xr9:uid="{2F907DDD-A922-407B-9ABA-EC188DF4B9FD}">
       <tableStyleElement type="headerRow" dxfId="48"/>
       <tableStyleElement type="firstRowStripe" dxfId="47"/>
       <tableStyleElement type="secondRowStripe" dxfId="46"/>
     </tableStyle>
-    <tableStyle name="2292-style" pivot="0" count="3" xr9:uid="{8BAD43FD-FA14-4A45-9804-DD91B474DCB4}">
+    <tableStyle name="2292-style" pivot="0" count="3" xr9:uid="{81A4B7C8-A71D-4583-A4C4-CE88E4BD30FB}">
       <tableStyleElement type="headerRow" dxfId="51"/>
       <tableStyleElement type="firstRowStripe" dxfId="50"/>
       <tableStyleElement type="secondRowStripe" dxfId="49"/>
     </tableStyle>
-    <tableStyle name="2293-style" pivot="0" count="3" xr9:uid="{DE622F4E-826F-4F17-BC9B-E4B0696C0946}">
+    <tableStyle name="2293-style" pivot="0" count="3" xr9:uid="{E4DAB688-7622-4D94-B5FE-85963BBD3E8E}">
       <tableStyleElement type="headerRow" dxfId="54"/>
       <tableStyleElement type="firstRowStripe" dxfId="53"/>
       <tableStyleElement type="secondRowStripe" dxfId="52"/>
@@ -1808,9 +1842,9 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4444444444444" defaultRowHeight="15" customHeight="1"/>
@@ -2177,89 +2211,131 @@
       <c r="Y9" s="16"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19"/>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="19"/>
-      <c r="Z10" s="19"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
+    <row r="10" ht="118.2" customHeight="1" spans="1:26">
+      <c r="A10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="16"/>
+    </row>
+    <row r="11" ht="118.2" customHeight="1" spans="1:26">
+      <c r="A11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+    </row>
+    <row r="12" ht="118.2" customHeight="1" spans="1:26">
+      <c r="A12" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16"/>
     </row>
     <row r="13" ht="15.75" customHeight="1" spans="1:26">
       <c r="A13" s="17"/>
@@ -29615,7 +29691,7 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F9 F4:F8">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F10 F11 F12 F4:F9">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>